<commit_message>
add finishing touches on index.html, add diagram image, add multi-line comment
</commit_message>
<xml_diff>
--- a/mis3371/homework1/mis3371-homework1-data-dictionary.xlsx
+++ b/mis3371/homework1/mis3371-homework1-data-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbcas\all-projects\DD-matt.github.io\mis3371\homework1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99CEFA27-3096-4EAD-8076-492905AE6DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32B7FCB-860C-4617-855E-3F682850FA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3310" yWindow="2670" windowWidth="16710" windowHeight="11110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Tables DD" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Function" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
   <si>
     <t>Table name</t>
   </si>
@@ -92,9 +91,6 @@
     <t>About</t>
   </si>
   <si>
-    <t>SessionID (Primary key)</t>
-  </si>
-  <si>
     <t>LoggedIn</t>
   </si>
   <si>
@@ -104,18 +100,6 @@
     <t>SignoutTime</t>
   </si>
   <si>
-    <t>RequestID (PK)</t>
-  </si>
-  <si>
-    <t>UserID (FK)</t>
-  </si>
-  <si>
-    <t>SessionID (FK)</t>
-  </si>
-  <si>
-    <t>FunctionID(FK)</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -150,16 +134,91 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>SessionID (PK)</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Table Name</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>0-20</t>
+  </si>
+  <si>
+    <t>0-50</t>
+  </si>
+  <si>
+    <t>[5-10]</t>
+  </si>
+  <si>
+    <t>"Male", "Female", "Other"</t>
+  </si>
+  <si>
+    <t>List of Languages</t>
+  </si>
+  <si>
+    <t>0-500</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>True, False</t>
+  </si>
+  <si>
+    <t>DateTime Object</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>timestamp when request is made</t>
+  </si>
+  <si>
+    <t>data that is posted or received</t>
+  </si>
+  <si>
+    <t>UserID (PK, FK)</t>
+  </si>
+  <si>
+    <t>SessionID (PK, FK)</t>
+  </si>
+  <si>
+    <t>FunctionID(PK, FK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,11 +252,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -236,7 +303,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F9229D56-E2F1-47B0-929D-BB5E70E6E631}" name="Table4" displayName="Table4" ref="A1:K5" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2448AB4F-1492-44A7-B468-C4FF1E9998F0}" name="Table7" displayName="Table7" ref="A1:E18" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E18" xr:uid="{2448AB4F-1492-44A7-B468-C4FF1E9998F0}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E086E028-FCCB-4D53-A819-9FB62970ACEE}" name="Column Name"/>
+    <tableColumn id="2" xr3:uid="{735B8785-9B57-4D3D-A79D-F0BA363149EA}" name="Table Name"/>
+    <tableColumn id="3" xr3:uid="{502BDD9C-62EE-4228-86AD-2CA4B410B863}" name="Data Type"/>
+    <tableColumn id="4" xr3:uid="{DD9513BC-1E1B-4229-99E2-C5B0A7143898}" name="Length" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2BE9E420-B004-410B-9B89-9D0E25F216EE}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F9229D56-E2F1-47B0-929D-BB5E70E6E631}" name="Table4" displayName="Table4" ref="A1:K5" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:K5" xr:uid="{F9229D56-E2F1-47B0-929D-BB5E70E6E631}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{2697E4AA-547D-41A0-8675-F404154D8829}" name="UserID (PK)"/>
@@ -255,11 +336,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{13FDE671-4227-4E7F-A60B-A58204D2BF88}" name="Table5" displayName="Table5" ref="A1:D5" totalsRowShown="0" headerRowDxfId="2">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{13FDE671-4227-4E7F-A60B-A58204D2BF88}" name="Table5" displayName="Table5" ref="A1:D5" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D5" xr:uid="{13FDE671-4227-4E7F-A60B-A58204D2BF88}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{64755451-79A1-49B9-8449-6C7BBD9BFF5D}" name="SessionID (Primary key)"/>
+    <tableColumn id="1" xr3:uid="{64755451-79A1-49B9-8449-6C7BBD9BFF5D}" name="SessionID (PK)"/>
     <tableColumn id="2" xr3:uid="{EF0E48DB-19D6-4EB7-81F0-36E1775DC20F}" name="LoggedIn"/>
     <tableColumn id="3" xr3:uid="{E70203F7-0F08-479F-9A80-1621D33C54B0}" name="LoginTime"/>
     <tableColumn id="4" xr3:uid="{5BC9A9F1-7835-48A4-9F3B-1916ED987879}" name="SignoutTime"/>
@@ -268,14 +349,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{628073BC-B28F-4798-A82B-80AC86D2F6B4}" name="Table6" displayName="Table6" ref="A1:F5" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:F5" xr:uid="{628073BC-B28F-4798-A82B-80AC86D2F6B4}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D8EBB50D-CEC7-4A27-9E18-9B081A48AD28}" name="RequestID (PK)"/>
-    <tableColumn id="2" xr3:uid="{2BA8DC55-C69C-41C1-9C25-4D4DCD5AAD6E}" name="UserID (FK)"/>
-    <tableColumn id="3" xr3:uid="{796CBDF1-DF57-4C83-A3B9-6811AF1CE4C8}" name="SessionID (FK)"/>
-    <tableColumn id="4" xr3:uid="{74046CAE-CF57-4711-85EA-087671865CE5}" name="FunctionID(FK)"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{628073BC-B28F-4798-A82B-80AC86D2F6B4}" name="Table6" displayName="Table6" ref="A1:E5" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:E5" xr:uid="{628073BC-B28F-4798-A82B-80AC86D2F6B4}"/>
+  <tableColumns count="5">
+    <tableColumn id="2" xr3:uid="{2BA8DC55-C69C-41C1-9C25-4D4DCD5AAD6E}" name="UserID (PK, FK)"/>
+    <tableColumn id="3" xr3:uid="{796CBDF1-DF57-4C83-A3B9-6811AF1CE4C8}" name="SessionID (PK, FK)"/>
+    <tableColumn id="4" xr3:uid="{74046CAE-CF57-4711-85EA-087671865CE5}" name="FunctionID(PK, FK)"/>
     <tableColumn id="5" xr3:uid="{6E604533-B9C0-401F-BBB3-F38900A3D378}" name="Time"/>
     <tableColumn id="6" xr3:uid="{BA963649-5603-4256-9150-602DE7A8D575}" name="Data"/>
   </tableColumns>
@@ -283,8 +363,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C638A3B-EA59-4259-B587-D996C318772B}" name="Table3" displayName="Table3" ref="A1:C5" totalsRowShown="0" headerRowDxfId="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C638A3B-EA59-4259-B587-D996C318772B}" name="Table3" displayName="Table3" ref="A1:C5" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:C5" xr:uid="{2C638A3B-EA59-4259-B587-D996C318772B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{114A6ABD-1200-45E4-AC7F-CA1DA2FC1F60}" name="FunctionID (PK)"/>
@@ -560,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,13 +686,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -628,7 +708,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <f>SUBTOTAL(109,Table1[Number of Columns])</f>
@@ -649,15 +729,282 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFED5FE-7467-48A2-A5EF-E08CCBF42368}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -666,7 +1013,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="E15:F15"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,16 +1031,16 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>9</v>
@@ -730,7 +1077,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,16 +1091,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -766,40 +1113,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B735B71-D6A8-4F41-B212-1615F0B45C24}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -814,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055474E6-E3C4-48A1-AA01-2F365A1C67F4}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,13 +1170,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>